<commit_message>
Atualizando texto do README
</commit_message>
<xml_diff>
--- a/tabs/tabelas_graficos.xlsx
+++ b/tabs/tabelas_graficos.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{9934F7EE-A292-4CC4-8FCD-BB10CF47BE9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EBCF1B45-8313-46A7-B5EA-B0E7D284C9DF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7F871319-D33C-4D47-91A4-A4FA8BFF2636}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{7F871319-D33C-4D47-91A4-A4FA8BFF2636}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico1" sheetId="9" r:id="rId1"/>
@@ -770,7 +770,7 @@
             <c:numRef>
               <c:f>[1]indice!$A$2:$A$1048576</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>40910</c:v>
@@ -14375,7 +14375,7 @@
             <c:numRef>
               <c:f>[1]indice!$A$2:$A$1048576</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>40910</c:v>
@@ -28257,7 +28257,7 @@
             <c:numRef>
               <c:f>[1]indice_mensal!$A$2:$A$1048576</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>40909</c:v>
@@ -28968,7 +28968,7 @@
             <c:numRef>
               <c:f>[1]indice_mensal!$A$2:$A$1048576</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>40909</c:v>
@@ -61817,7 +61817,7 @@
   <dimension ref="B2:P34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63935,7 +63935,7 @@
   <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adicionando documentos para o site
</commit_message>
<xml_diff>
--- a/tabs/tabelas_graficos.xlsx
+++ b/tabs/tabelas_graficos.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{9934F7EE-A292-4CC4-8FCD-BB10CF47BE9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EBCF1B45-8313-46A7-B5EA-B0E7D284C9DF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{7F871319-D33C-4D47-91A4-A4FA8BFF2636}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7F871319-D33C-4D47-91A4-A4FA8BFF2636}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico1" sheetId="9" r:id="rId1"/>
@@ -770,7 +770,7 @@
             <c:numRef>
               <c:f>[1]indice!$A$2:$A$1048576</c:f>
               <c:numCache>
-                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>40910</c:v>
@@ -7548,6 +7548,9 @@
                 </c:pt>
                 <c:pt idx="2258">
                   <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="2259">
+                  <c:v>44249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14108,7 +14111,7 @@
                   <c:v>441.98452943191631</c:v>
                 </c:pt>
                 <c:pt idx="2183">
-                  <c:v>442.87142749621847</c:v>
+                  <c:v>442.94962006988891</c:v>
                 </c:pt>
                 <c:pt idx="2184">
                   <c:v>449.18139226999358</c:v>
@@ -14135,7 +14138,7 @@
                   <c:v>461.0083478981071</c:v>
                 </c:pt>
                 <c:pt idx="2192">
-                  <c:v>464.26100220677438</c:v>
+                  <c:v>464.92872643983861</c:v>
                 </c:pt>
                 <c:pt idx="2193">
                   <c:v>458.24641857487768</c:v>
@@ -14150,7 +14153,7 @@
                   <c:v>460.39521771313167</c:v>
                 </c:pt>
                 <c:pt idx="2197">
-                  <c:v>477.9550546184467</c:v>
+                  <c:v>478.5974636132612</c:v>
                 </c:pt>
                 <c:pt idx="2198">
                   <c:v>473.02708697651252</c:v>
@@ -14177,7 +14180,7 @@
                   <c:v>474.99825648205581</c:v>
                 </c:pt>
                 <c:pt idx="2206">
-                  <c:v>478.47731679869531</c:v>
+                  <c:v>478.32753321870251</c:v>
                 </c:pt>
                 <c:pt idx="2207">
                   <c:v>481.84373506144158</c:v>
@@ -14192,7 +14195,7 @@
                   <c:v>466.49760462989622</c:v>
                 </c:pt>
                 <c:pt idx="2211">
-                  <c:v>469.90305089764678</c:v>
+                  <c:v>470.20843458214023</c:v>
                 </c:pt>
                 <c:pt idx="2212">
                   <c:v>461.56959130668321</c:v>
@@ -14207,7 +14210,7 @@
                   <c:v>470.78426837469777</c:v>
                 </c:pt>
                 <c:pt idx="2216">
-                  <c:v>470.60778046489798</c:v>
+                  <c:v>470.78573487455873</c:v>
                 </c:pt>
                 <c:pt idx="2217">
                   <c:v>466.58383533336848</c:v>
@@ -14222,7 +14225,7 @@
                   <c:v>474.30996970436058</c:v>
                 </c:pt>
                 <c:pt idx="2221">
-                  <c:v>468.39712080325131</c:v>
+                  <c:v>468.68339885494231</c:v>
                 </c:pt>
                 <c:pt idx="2222">
                   <c:v>467.8960809463469</c:v>
@@ -14255,7 +14258,7 @@
                   <c:v>467.05378774932512</c:v>
                 </c:pt>
                 <c:pt idx="2232">
-                  <c:v>505.54701856530221</c:v>
+                  <c:v>505.95114565933068</c:v>
                 </c:pt>
                 <c:pt idx="2233">
                   <c:v>530.92910717282791</c:v>
@@ -14270,7 +14273,7 @@
                   <c:v>516.78221053458935</c:v>
                 </c:pt>
                 <c:pt idx="2237">
-                  <c:v>523.17718863678374</c:v>
+                  <c:v>519.518619745715</c:v>
                 </c:pt>
                 <c:pt idx="2238">
                   <c:v>527.52134391191521</c:v>
@@ -14285,7 +14288,7 @@
                   <c:v>520.34309004879549</c:v>
                 </c:pt>
                 <c:pt idx="2242">
-                  <c:v>512.33584825789535</c:v>
+                  <c:v>511.43316415724632</c:v>
                 </c:pt>
                 <c:pt idx="2243">
                   <c:v>514.91306160363206</c:v>
@@ -14297,7 +14300,7 @@
                   <c:v>508.87779311710273</c:v>
                 </c:pt>
                 <c:pt idx="2246">
-                  <c:v>494.03442088230048</c:v>
+                  <c:v>490.2008555654474</c:v>
                 </c:pt>
                 <c:pt idx="2247">
                   <c:v>504.16750263001148</c:v>
@@ -14312,7 +14315,7 @@
                   <c:v>524.13582833129362</c:v>
                 </c:pt>
                 <c:pt idx="2251">
-                  <c:v>532.28465914264518</c:v>
+                  <c:v>530.10770024967235</c:v>
                 </c:pt>
                 <c:pt idx="2252">
                   <c:v>521.36381083943934</c:v>
@@ -14327,13 +14330,16 @@
                   <c:v>513.505252331257</c:v>
                 </c:pt>
                 <c:pt idx="2256">
-                  <c:v>506.02501970460531</c:v>
+                  <c:v>506.39178297318688</c:v>
                 </c:pt>
                 <c:pt idx="2257">
                   <c:v>494.13280592721168</c:v>
                 </c:pt>
                 <c:pt idx="2258">
-                  <c:v>492.49561126113719</c:v>
+                  <c:v>495.86956575069809</c:v>
+                </c:pt>
+                <c:pt idx="2259">
+                  <c:v>490.92836344505719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14375,7 +14381,7 @@
             <c:numRef>
               <c:f>[1]indice!$A$2:$A$1048576</c:f>
               <c:numCache>
-                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>40910</c:v>
@@ -21153,6 +21159,9 @@
                 </c:pt>
                 <c:pt idx="2258">
                   <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="2259">
+                  <c:v>44249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -27860,7 +27869,7 @@
                   <c:v>214.88529442858649</c:v>
                 </c:pt>
                 <c:pt idx="2232">
-                  <c:v>220.5994291151284</c:v>
+                  <c:v>220.38446629312469</c:v>
                 </c:pt>
                 <c:pt idx="2233">
                   <c:v>216.38474821157979</c:v>
@@ -27878,7 +27887,7 @@
                   <c:v>212.32336046798471</c:v>
                 </c:pt>
                 <c:pt idx="2238">
-                  <c:v>212.32336046798471</c:v>
+                  <c:v>213.62723332276141</c:v>
                 </c:pt>
                 <c:pt idx="2239">
                   <c:v>212.62466081685869</c:v>
@@ -27939,6 +27948,9 @@
                 </c:pt>
                 <c:pt idx="2258">
                   <c:v>209.2328294040949</c:v>
+                </c:pt>
+                <c:pt idx="2259">
+                  <c:v>198.51992811079401</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -28257,7 +28269,7 @@
             <c:numRef>
               <c:f>[1]indice_mensal!$A$2:$A$1048576</c:f>
               <c:numCache>
-                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>40909</c:v>
@@ -28923,10 +28935,10 @@
                   <c:v>476.76924650405431</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>494.03442088230048</c:v>
+                  <c:v>490.2008555654474</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>492.49561126113719</c:v>
+                  <c:v>490.92836344505719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -28968,7 +28980,7 @@
             <c:numRef>
               <c:f>[1]indice_mensal!$A$2:$A$1048576</c:f>
               <c:numCache>
-                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
                   <c:v>40909</c:v>
@@ -29637,7 +29649,7 @@
                   <c:v>204.40321387038799</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>209.2328294040949</c:v>
+                  <c:v>198.51992811079401</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -30028,34 +30040,34 @@
                 <c:formatCode>#,##0.0000_ ;[Red]\-#,##0.0000\ </c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.505</c:v>
+                  <c:v>0.50639999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0178</c:v>
+                  <c:v>1.0202</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85019999999999996</c:v>
+                  <c:v>0.88780000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75509999999999999</c:v>
+                  <c:v>0.75419999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.66790000000000005</c:v>
+                  <c:v>0.68030000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.6</c:v>
+                  <c:v>0.60429999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.57750000000000001</c:v>
+                  <c:v>0.5867</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.41360000000000002</c:v>
+                  <c:v>0.42349999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3921</c:v>
+                  <c:v>0.4047</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.13489999999999999</c:v>
+                  <c:v>0.1085</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -30603,31 +30615,31 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.44594160118704962</c:v>
+                  <c:v>0.44157922994593263</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26563233582364709</c:v>
+                  <c:v>0.27508010891412737</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.3772928729853864E-2</c:v>
+                  <c:v>6.2110276675833097E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.1870521812547428E-2</c:v>
+                  <c:v>5.0547434655360747E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0121657557831122E-2</c:v>
+                  <c:v>5.018229588233817E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9800668158157901E-2</c:v>
+                  <c:v>3.9129173899198538E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2746680769462758E-2</c:v>
+                  <c:v>3.2161247099097387E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.613960916092696E-2</c:v>
+                  <c:v>2.5159701144226429E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3973996800523319E-2</c:v>
+                  <c:v>2.4050531783885581E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -34138,22 +34150,22 @@
         </row>
         <row r="2">
           <cell r="A2">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B2" t="str">
             <v>Índice</v>
           </cell>
           <cell r="C2">
-            <v>-3.1147822016431852E-3</v>
+            <v>1.484101611309185E-3</v>
           </cell>
           <cell r="D2">
-            <v>3.2985275104042033E-2</v>
+            <v>2.969805004166215E-2</v>
           </cell>
           <cell r="E2">
-            <v>0.823260256374581</v>
+            <v>0.81745817288467659</v>
           </cell>
           <cell r="F2">
-            <v>1.1047236094480439</v>
+            <v>1.0980258371127469</v>
           </cell>
           <cell r="G2">
             <v>0.63504395478950859</v>
@@ -34183,27 +34195,27 @@
             <v>8.5909097291277492E-2</v>
           </cell>
           <cell r="P2">
-            <v>3.2985275104041811E-2</v>
+            <v>2.969805004166215E-2</v>
           </cell>
         </row>
         <row r="3">
           <cell r="A3">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B3" t="str">
             <v>Ibovespa</v>
           </cell>
           <cell r="C3">
-            <v>2.3627884524209719E-2</v>
+            <v>-2.8782745868783929E-2</v>
           </cell>
           <cell r="D3">
-            <v>-4.6770489329955867E-3</v>
+            <v>-5.5638442324778208E-2</v>
           </cell>
           <cell r="E3">
-            <v>0.2423418145296283</v>
+            <v>0.17873284231670561</v>
           </cell>
           <cell r="F3">
-            <v>0.78134469412859087</v>
+            <v>0.69013830968167933</v>
           </cell>
           <cell r="G3">
             <v>7.3968354653416446E-2</v>
@@ -34233,27 +34245,27 @@
             <v>2.8819288744782678E-2</v>
           </cell>
           <cell r="P3">
-            <v>-4.6770489329956977E-3</v>
+            <v>-5.5638442324778097E-2</v>
           </cell>
         </row>
         <row r="4">
           <cell r="A4">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B4" t="str">
             <v>BNBR3.SA</v>
           </cell>
           <cell r="C4">
-            <v>-2.926491065922077E-2</v>
+            <v>-4.9653274608967291E-2</v>
           </cell>
           <cell r="D4">
-            <v>-7.9078973684210574E-2</v>
+            <v>-9.8421092105263064E-2</v>
           </cell>
           <cell r="E4">
-            <v>0.55533328888888867</v>
+            <v>0.52266659999999998</v>
           </cell>
           <cell r="F4">
-            <v>1.473144893043989</v>
+            <v>1.421201392975314</v>
           </cell>
           <cell r="G4">
             <v>-0.45714285714285718</v>
@@ -34283,12 +34295,12 @@
             <v>-0.19991576376283329</v>
           </cell>
           <cell r="P4">
-            <v>-7.9078973684210574E-2</v>
+            <v>-9.8421092105263064E-2</v>
           </cell>
         </row>
         <row r="5">
           <cell r="A5">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B5" t="str">
             <v>COCE3.SA</v>
@@ -34338,22 +34350,22 @@
         </row>
         <row r="6">
           <cell r="A6">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B6" t="str">
             <v>COCE5.SA</v>
           </cell>
           <cell r="C6">
-            <v>-2.5393384313068149E-2</v>
+            <v>-5.4259358758195757E-2</v>
           </cell>
           <cell r="D6">
-            <v>-9.1666666666666674E-2</v>
+            <v>-0.1284999833333334</v>
           </cell>
           <cell r="E6">
-            <v>-9.0909090909092605E-3</v>
+            <v>-4.9272709090909313E-2</v>
           </cell>
           <cell r="F6">
-            <v>0.16577540106951871</v>
+            <v>0.1185026951871657</v>
           </cell>
           <cell r="G6">
             <v>0.30624089096543128</v>
@@ -34383,27 +34395,27 @@
             <v>-3.8615606473321518E-2</v>
           </cell>
           <cell r="P6">
-            <v>-9.1666666666666674E-2</v>
+            <v>-0.1284999833333334</v>
           </cell>
         </row>
         <row r="7">
           <cell r="A7">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B7" t="str">
             <v>GRND3.SA</v>
           </cell>
           <cell r="C7">
-            <v>-1.156812339331614E-2</v>
+            <v>-3.1128404669260701E-2</v>
           </cell>
           <cell r="D7">
-            <v>-8.2338902147971349E-2</v>
+            <v>-0.10859188544152749</v>
           </cell>
           <cell r="E7">
-            <v>-0.11303344867358719</v>
+            <v>-0.1384083044982701</v>
           </cell>
           <cell r="F7">
-            <v>0.15407709625198021</v>
+            <v>0.1210605863462018</v>
           </cell>
           <cell r="G7">
             <v>1.14434332176116</v>
@@ -34433,27 +34445,27 @@
             <v>-0.31758957654723119</v>
           </cell>
           <cell r="P7">
-            <v>-8.2338902147971349E-2</v>
+            <v>-0.10859188544152749</v>
           </cell>
         </row>
         <row r="8">
           <cell r="A8">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B8" t="str">
             <v>MDIA3.SA</v>
           </cell>
           <cell r="C8">
-            <v>-2.2890778286460689E-3</v>
+            <v>-1.725275438794804E-2</v>
           </cell>
           <cell r="D8">
-            <v>-0.1042278595352948</v>
+            <v>-0.13035818759958351</v>
           </cell>
           <cell r="E8">
-            <v>-0.35057471264367812</v>
+            <v>-0.36951892294593452</v>
           </cell>
           <cell r="F8">
-            <v>-0.3376989773907233</v>
+            <v>-0.35701878230128492</v>
           </cell>
           <cell r="G8">
             <v>0.63710698113207531</v>
@@ -34483,27 +34495,27 @@
             <v>-0.10720840853429051</v>
           </cell>
           <cell r="P8">
-            <v>-0.1042278595352948</v>
+            <v>-0.13035818759958351</v>
           </cell>
         </row>
         <row r="9">
           <cell r="A9">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B9" t="str">
             <v>HAPV3.SA</v>
           </cell>
           <cell r="C9">
-            <v>-2.2413793103448151E-2</v>
+            <v>-2.213156668608041E-2</v>
           </cell>
           <cell r="D9">
-            <v>0.1146788990825689</v>
+            <v>0.1002621887287025</v>
           </cell>
           <cell r="E9">
-            <v>1.609696225836146</v>
+            <v>1.57594369438478</v>
           </cell>
           <cell r="F9">
-            <v>2.081521739130435</v>
+            <v>2.0416668478260869</v>
           </cell>
           <cell r="M9">
             <v>0.13043478260869579</v>
@@ -34515,27 +34527,27 @@
             <v>0.19405320813771529</v>
           </cell>
           <cell r="P9">
-            <v>0.1146788990825689</v>
+            <v>0.1002621887287025</v>
           </cell>
         </row>
         <row r="10">
           <cell r="A10">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B10" t="str">
             <v>ARCE</v>
           </cell>
           <cell r="C10">
-            <v>0.1014074814136892</v>
+            <v>0.13695173309160041</v>
           </cell>
           <cell r="D10">
-            <v>3.6490608118537222E-2</v>
+            <v>6.9939884302379518E-2</v>
           </cell>
           <cell r="E10">
-            <v>1.122930353619811</v>
+            <v>1.1914408477440079</v>
           </cell>
           <cell r="F10">
-            <v>1.3747996346313229</v>
+            <v>1.451438369452339</v>
           </cell>
           <cell r="M10">
             <v>3.6850058535654817E-2</v>
@@ -34547,59 +34559,59 @@
             <v>2.5537255795764709E-2</v>
           </cell>
           <cell r="P10">
-            <v>3.6490608118537222E-2</v>
+            <v>6.9939884302379518E-2</v>
           </cell>
         </row>
         <row r="11">
           <cell r="A11">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B11" t="str">
             <v>PGMN3.SA</v>
           </cell>
           <cell r="C11">
-            <v>-1.477832512315269E-2</v>
+            <v>-3.4482758620689613E-2</v>
           </cell>
           <cell r="D11">
-            <v>0.1086474501108647</v>
+            <v>8.6474501108647628E-2</v>
           </cell>
           <cell r="E11">
-            <v>6.6098081023453936E-2</v>
+            <v>4.4776119402985197E-2</v>
           </cell>
           <cell r="F11">
-            <v>6.6098081023453936E-2</v>
+            <v>4.4776119402985197E-2</v>
           </cell>
           <cell r="O11">
             <v>-3.8379530916844429E-2</v>
           </cell>
           <cell r="P11">
-            <v>0.1086474501108647</v>
+            <v>8.6474501108647628E-2</v>
           </cell>
         </row>
         <row r="12">
           <cell r="A12">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B12" t="str">
             <v>AERI3.SA</v>
           </cell>
           <cell r="C12">
-            <v>-0.14527027027027031</v>
+            <v>-0.1469594594594594</v>
           </cell>
           <cell r="D12">
-            <v>1.2000000000000011E-2</v>
+            <v>1.0000000000000011E-2</v>
           </cell>
           <cell r="E12">
-            <v>0.51724137931034453</v>
+            <v>0.5142428785607196</v>
           </cell>
           <cell r="F12">
-            <v>0.51724137931034453</v>
+            <v>0.5142428785607196</v>
           </cell>
           <cell r="O12">
             <v>0.49925037481259382</v>
           </cell>
           <cell r="P12">
-            <v>1.2000000000000011E-2</v>
+            <v>1.0000000000000011E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -34629,16 +34641,16 @@
         </row>
         <row r="3">
           <cell r="B3">
-            <v>1.4800000000000001E-2</v>
+            <v>1.37E-2</v>
           </cell>
           <cell r="C3">
-            <v>7.22E-2</v>
+            <v>7.2499999999999995E-2</v>
           </cell>
           <cell r="D3">
-            <v>4.8783783783783781</v>
+            <v>5.2919708029197077</v>
           </cell>
           <cell r="E3">
-            <v>5.1999999999999998E-3</v>
+            <v>5.3E-3</v>
           </cell>
           <cell r="F3">
             <v>48</v>
@@ -34655,16 +34667,16 @@
             <v>BNBR3.SA</v>
           </cell>
           <cell r="B4">
-            <v>2.69E-2</v>
+            <v>2.64E-2</v>
           </cell>
           <cell r="C4">
-            <v>0.13900000000000001</v>
+            <v>0.13919999999999999</v>
           </cell>
           <cell r="D4">
-            <v>5.1672862453531598</v>
+            <v>5.2727272727272734</v>
           </cell>
           <cell r="E4">
-            <v>1.9300000000000001E-2</v>
+            <v>1.9400000000000001E-2</v>
           </cell>
           <cell r="F4">
             <v>48</v>
@@ -34707,16 +34719,16 @@
             <v>COCE5.SA</v>
           </cell>
           <cell r="B6">
-            <v>5.5999999999999999E-3</v>
+            <v>4.7999999999999996E-3</v>
           </cell>
           <cell r="C6">
-            <v>6.7100000000000007E-2</v>
+            <v>6.7799999999999999E-2</v>
           </cell>
           <cell r="D6">
-            <v>11.982142857142859</v>
+            <v>14.125</v>
           </cell>
           <cell r="E6">
-            <v>4.4999999999999997E-3</v>
+            <v>4.5999999999999999E-3</v>
           </cell>
           <cell r="F6">
             <v>48</v>
@@ -34733,16 +34745,16 @@
             <v>GRND3.SA</v>
           </cell>
           <cell r="B7">
+            <v>5.7000000000000002E-3</v>
+          </cell>
+          <cell r="C7">
+            <v>7.9399999999999998E-2</v>
+          </cell>
+          <cell r="D7">
+            <v>13.92982456140351</v>
+          </cell>
+          <cell r="E7">
             <v>6.3E-3</v>
-          </cell>
-          <cell r="C7">
-            <v>7.9000000000000001E-2</v>
-          </cell>
-          <cell r="D7">
-            <v>12.53968253968254</v>
-          </cell>
-          <cell r="E7">
-            <v>6.1999999999999998E-3</v>
           </cell>
           <cell r="F7">
             <v>48</v>
@@ -34759,16 +34771,16 @@
             <v>MDIA3.SA</v>
           </cell>
           <cell r="B8">
-            <v>-3.5000000000000001E-3</v>
+            <v>-4.1000000000000003E-3</v>
           </cell>
           <cell r="C8">
-            <v>9.2899999999999996E-2</v>
+            <v>9.3200000000000005E-2</v>
           </cell>
           <cell r="D8">
-            <v>-26.542857142857141</v>
+            <v>-22.73170731707317</v>
           </cell>
           <cell r="E8">
-            <v>8.6E-3</v>
+            <v>8.6999999999999994E-3</v>
           </cell>
           <cell r="F8">
             <v>48</v>
@@ -34785,16 +34797,16 @@
             <v>HAPV3.SA</v>
           </cell>
           <cell r="B9">
-            <v>3.85E-2</v>
+            <v>3.7999999999999999E-2</v>
           </cell>
           <cell r="C9">
-            <v>0.10059999999999999</v>
+            <v>0.1002</v>
           </cell>
           <cell r="D9">
-            <v>2.6129870129870132</v>
+            <v>2.6368421052631579</v>
           </cell>
           <cell r="E9">
-            <v>1.01E-2</v>
+            <v>0.01</v>
           </cell>
           <cell r="F9">
             <v>34</v>
@@ -34811,16 +34823,16 @@
             <v>ARCE</v>
           </cell>
           <cell r="B10">
-            <v>3.9399999999999998E-2</v>
+            <v>4.0599999999999997E-2</v>
           </cell>
           <cell r="C10">
-            <v>0.14080000000000001</v>
+            <v>0.14149999999999999</v>
           </cell>
           <cell r="D10">
-            <v>3.5736040609137061</v>
+            <v>3.485221674876847</v>
           </cell>
           <cell r="E10">
-            <v>1.9800000000000002E-2</v>
+            <v>0.02</v>
           </cell>
           <cell r="F10">
             <v>29</v>
@@ -34837,22 +34849,22 @@
             <v>PGMN3.SA</v>
           </cell>
           <cell r="B11">
-            <v>1.37E-2</v>
+            <v>1.03E-2</v>
           </cell>
           <cell r="C11">
-            <v>8.5000000000000006E-2</v>
+            <v>8.5199999999999998E-2</v>
           </cell>
           <cell r="D11">
-            <v>6.2043795620437958</v>
+            <v>8.2718446601941746</v>
           </cell>
           <cell r="E11">
-            <v>7.1999999999999998E-3</v>
+            <v>7.3000000000000001E-3</v>
           </cell>
           <cell r="F11">
             <v>6</v>
           </cell>
           <cell r="G11">
-            <v>0.12970000000000001</v>
+            <v>0.12529999999999999</v>
           </cell>
           <cell r="H11">
             <v>-0.1087</v>
@@ -34863,16 +34875,16 @@
             <v>AERI3.SA</v>
           </cell>
           <cell r="B12">
-            <v>0.13469999999999999</v>
+            <v>0.13450000000000001</v>
           </cell>
           <cell r="C12">
-            <v>0.27989999999999998</v>
+            <v>0.28100000000000003</v>
           </cell>
           <cell r="D12">
-            <v>2.077951002227171</v>
+            <v>2.0892193308550189</v>
           </cell>
           <cell r="E12">
-            <v>7.8299999999999995E-2</v>
+            <v>7.9000000000000001E-2</v>
           </cell>
           <cell r="F12">
             <v>4</v>
@@ -34881,29 +34893,29 @@
             <v>0.50380000000000003</v>
           </cell>
           <cell r="H12">
-            <v>-0.14380000000000001</v>
+            <v>-0.14699999999999999</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2">
         <row r="2">
           <cell r="B2">
-            <v>0.13070000000000001</v>
+            <v>0.13689999999999999</v>
           </cell>
           <cell r="C2">
-            <v>1.03E-2</v>
+            <v>1.0699999999999999E-2</v>
           </cell>
           <cell r="D2">
-            <v>0.505</v>
+            <v>0.50639999999999996</v>
           </cell>
           <cell r="E2">
-            <v>0.55220000000000002</v>
+            <v>0.55630000000000002</v>
           </cell>
           <cell r="F2">
             <v>0</v>
           </cell>
           <cell r="G2">
-            <v>0.30499999999999999</v>
+            <v>0.3095</v>
           </cell>
         </row>
         <row r="3">
@@ -34911,22 +34923,22 @@
             <v>BNBR3.SA</v>
           </cell>
           <cell r="B3">
-            <v>0.28439999999999999</v>
+            <v>0.28179999999999999</v>
           </cell>
           <cell r="C3">
-            <v>2.1100000000000001E-2</v>
+            <v>2.0899999999999998E-2</v>
           </cell>
           <cell r="D3">
-            <v>0.3921</v>
+            <v>0.4047</v>
           </cell>
           <cell r="E3">
-            <v>0.20369999999999999</v>
+            <v>0.21079999999999999</v>
           </cell>
           <cell r="F3">
-            <v>0.1648</v>
+            <v>0.15049999999999999</v>
           </cell>
           <cell r="G3">
-            <v>4.1500000000000002E-2</v>
+            <v>4.4400000000000002E-2</v>
           </cell>
         </row>
         <row r="4">
@@ -34934,22 +34946,22 @@
             <v>COCE3.SA</v>
           </cell>
           <cell r="B4">
-            <v>-1.0200000000000001E-2</v>
+            <v>-5.1999999999999998E-3</v>
           </cell>
           <cell r="C4">
-            <v>-8.9999999999999998E-4</v>
+            <v>-4.0000000000000002E-4</v>
           </cell>
           <cell r="D4">
-            <v>0.85019999999999996</v>
+            <v>0.88780000000000003</v>
           </cell>
           <cell r="E4">
-            <v>0.47570000000000001</v>
+            <v>0.4985</v>
           </cell>
           <cell r="F4">
-            <v>5.9999999999999995E-4</v>
+            <v>2.9999999999999997E-4</v>
           </cell>
           <cell r="G4">
-            <v>0.2263</v>
+            <v>0.2485</v>
           </cell>
         </row>
         <row r="5">
@@ -34957,22 +34969,22 @@
             <v>COCE5.SA</v>
           </cell>
           <cell r="B5">
-            <v>-3.4599999999999999E-2</v>
+            <v>-3.8300000000000001E-2</v>
           </cell>
           <cell r="C5">
-            <v>-2.8999999999999998E-3</v>
+            <v>-3.2000000000000002E-3</v>
           </cell>
           <cell r="D5">
-            <v>0.57750000000000001</v>
+            <v>0.5867</v>
           </cell>
           <cell r="E5">
-            <v>0.62150000000000005</v>
+            <v>0.62739999999999996</v>
           </cell>
           <cell r="F5">
             <v>0</v>
           </cell>
           <cell r="G5">
-            <v>0.38629999999999998</v>
+            <v>0.39369999999999999</v>
           </cell>
         </row>
         <row r="6">
@@ -34980,22 +34992,22 @@
             <v>GRND3.SA</v>
           </cell>
           <cell r="B6">
-            <v>-3.0700000000000002E-2</v>
+            <v>-3.0599999999999999E-2</v>
           </cell>
           <cell r="C6">
             <v>-2.5999999999999999E-3</v>
           </cell>
           <cell r="D6">
-            <v>0.6</v>
+            <v>0.60429999999999995</v>
           </cell>
           <cell r="E6">
-            <v>0.54820000000000002</v>
+            <v>0.55179999999999996</v>
           </cell>
           <cell r="F6">
-            <v>1E-4</v>
+            <v>0</v>
           </cell>
           <cell r="G6">
-            <v>0.30049999999999999</v>
+            <v>0.30449999999999999</v>
           </cell>
         </row>
         <row r="7">
@@ -35003,22 +35015,22 @@
             <v>MDIA3.SA</v>
           </cell>
           <cell r="B7">
-            <v>-0.16209999999999999</v>
+            <v>-0.1595</v>
           </cell>
           <cell r="C7">
-            <v>-1.46E-2</v>
+            <v>-1.44E-2</v>
           </cell>
           <cell r="D7">
-            <v>0.75509999999999999</v>
+            <v>0.75419999999999998</v>
           </cell>
           <cell r="E7">
-            <v>0.58720000000000006</v>
+            <v>0.58650000000000002</v>
           </cell>
           <cell r="F7">
             <v>0</v>
           </cell>
           <cell r="G7">
-            <v>0.3448</v>
+            <v>0.34399999999999997</v>
           </cell>
         </row>
         <row r="8">
@@ -35026,22 +35038,22 @@
             <v>HAPV3.SA</v>
           </cell>
           <cell r="B8">
-            <v>0.42209999999999998</v>
+            <v>0.42970000000000003</v>
           </cell>
           <cell r="C8">
-            <v>2.98E-2</v>
+            <v>3.0200000000000001E-2</v>
           </cell>
           <cell r="D8">
-            <v>0.66790000000000005</v>
+            <v>0.68030000000000002</v>
           </cell>
           <cell r="E8">
-            <v>0.54139999999999999</v>
+            <v>0.55579999999999996</v>
           </cell>
           <cell r="F8">
-            <v>8.9999999999999998E-4</v>
+            <v>5.9999999999999995E-4</v>
           </cell>
           <cell r="G8">
-            <v>0.29310000000000003</v>
+            <v>0.30890000000000001</v>
           </cell>
         </row>
         <row r="9">
@@ -35049,22 +35061,22 @@
             <v>ARCE_Ibovespa</v>
           </cell>
           <cell r="B9">
-            <v>0.54630000000000001</v>
+            <v>0.58040000000000003</v>
           </cell>
           <cell r="C9">
-            <v>3.6999999999999998E-2</v>
+            <v>3.8899999999999997E-2</v>
           </cell>
           <cell r="D9">
-            <v>0.13489999999999999</v>
+            <v>0.1085</v>
           </cell>
           <cell r="E9">
-            <v>7.9299999999999995E-2</v>
+            <v>6.3799999999999996E-2</v>
           </cell>
           <cell r="F9">
-            <v>0.68269999999999997</v>
+            <v>0.74239999999999995</v>
           </cell>
           <cell r="G9">
-            <v>6.3E-3</v>
+            <v>4.1000000000000003E-3</v>
           </cell>
         </row>
         <row r="10">
@@ -35072,22 +35084,22 @@
             <v>ARCE_SP500</v>
           </cell>
           <cell r="B10">
-            <v>0.1348</v>
+            <v>0.1439</v>
           </cell>
           <cell r="C10">
-            <v>1.06E-2</v>
+            <v>1.1299999999999999E-2</v>
           </cell>
           <cell r="D10">
-            <v>1.0178</v>
+            <v>1.0202</v>
           </cell>
           <cell r="E10">
-            <v>0.43540000000000001</v>
+            <v>0.43409999999999999</v>
           </cell>
           <cell r="F10">
-            <v>1.6199999999999999E-2</v>
+            <v>1.6500000000000001E-2</v>
           </cell>
           <cell r="G10">
-            <v>0.18959999999999999</v>
+            <v>0.18840000000000001</v>
           </cell>
         </row>
         <row r="11">
@@ -35095,22 +35107,22 @@
             <v>PGMN3.SA</v>
           </cell>
           <cell r="B11">
-            <v>-0.17519999999999999</v>
+            <v>-0.17430000000000001</v>
           </cell>
           <cell r="C11">
-            <v>-1.5900000000000001E-2</v>
+            <v>-1.5800000000000002E-2</v>
           </cell>
           <cell r="D11">
-            <v>0.41360000000000002</v>
+            <v>0.42349999999999999</v>
           </cell>
           <cell r="E11">
-            <v>0.33310000000000001</v>
+            <v>0.35520000000000002</v>
           </cell>
           <cell r="F11">
-            <v>0.51880000000000004</v>
+            <v>0.48970000000000002</v>
           </cell>
           <cell r="G11">
-            <v>0.1109</v>
+            <v>0.12609999999999999</v>
           </cell>
         </row>
       </sheetData>
@@ -59141,7 +59153,7 @@
             <v>44127</v>
           </cell>
           <cell r="D2185">
-            <v>442.87142749621847</v>
+            <v>442.94962006988891</v>
           </cell>
           <cell r="E2185">
             <v>178.41914226310041</v>
@@ -59240,7 +59252,7 @@
             <v>44141</v>
           </cell>
           <cell r="D2194">
-            <v>464.26100220677438</v>
+            <v>464.92872643983861</v>
           </cell>
           <cell r="E2194">
             <v>177.6068647143814</v>
@@ -59295,7 +59307,7 @@
             <v>44148</v>
           </cell>
           <cell r="D2199">
-            <v>477.9550546184467</v>
+            <v>478.5974636132612</v>
           </cell>
           <cell r="E2199">
             <v>184.14913486274099</v>
@@ -59394,7 +59406,7 @@
             <v>44162</v>
           </cell>
           <cell r="D2208">
-            <v>478.47731679869531</v>
+            <v>478.32753321870251</v>
           </cell>
           <cell r="E2208">
             <v>194.8320823201889</v>
@@ -59449,7 +59461,7 @@
             <v>44169</v>
           </cell>
           <cell r="D2213">
-            <v>469.90305089764678</v>
+            <v>470.20843458214023</v>
           </cell>
           <cell r="E2213">
             <v>200.30658631990701</v>
@@ -59504,7 +59516,7 @@
             <v>44176</v>
           </cell>
           <cell r="D2218">
-            <v>470.60778046489798</v>
+            <v>470.78573487455873</v>
           </cell>
           <cell r="E2218">
             <v>203.19801247489161</v>
@@ -59559,7 +59571,7 @@
             <v>44183</v>
           </cell>
           <cell r="D2223">
-            <v>468.39712080325131</v>
+            <v>468.68339885494231</v>
           </cell>
           <cell r="E2223">
             <v>207.34926172604571</v>
@@ -59680,10 +59692,10 @@
             <v>44204</v>
           </cell>
           <cell r="D2234">
-            <v>505.54701856530221</v>
+            <v>505.95114565933068</v>
           </cell>
           <cell r="E2234">
-            <v>220.5994291151284</v>
+            <v>220.38446629312469</v>
           </cell>
         </row>
         <row r="2235">
@@ -59735,7 +59747,7 @@
             <v>44211</v>
           </cell>
           <cell r="D2239">
-            <v>523.17718863678374</v>
+            <v>519.518619745715</v>
           </cell>
           <cell r="E2239">
             <v>212.32336046798471</v>
@@ -59749,7 +59761,7 @@
             <v>527.52134391191521</v>
           </cell>
           <cell r="E2240">
-            <v>212.32336046798471</v>
+            <v>213.62723332276141</v>
           </cell>
         </row>
         <row r="2241">
@@ -59790,7 +59802,7 @@
             <v>44218</v>
           </cell>
           <cell r="D2244">
-            <v>512.33584825789535</v>
+            <v>511.43316415724632</v>
           </cell>
           <cell r="E2244">
             <v>206.45593262148921</v>
@@ -59834,7 +59846,7 @@
             <v>44225</v>
           </cell>
           <cell r="D2248">
-            <v>494.03442088230048</v>
+            <v>490.2008555654474</v>
           </cell>
           <cell r="E2248">
             <v>204.40321387038799</v>
@@ -59889,7 +59901,7 @@
             <v>44232</v>
           </cell>
           <cell r="D2253">
-            <v>532.28465914264518</v>
+            <v>530.10770024967235</v>
           </cell>
           <cell r="E2253">
             <v>211.3066920393276</v>
@@ -59944,7 +59956,7 @@
             <v>44239</v>
           </cell>
           <cell r="D2258">
-            <v>506.02501970460531</v>
+            <v>506.39178297318688</v>
           </cell>
           <cell r="E2258">
             <v>209.88124185079471</v>
@@ -59966,10 +59978,21 @@
             <v>44246</v>
           </cell>
           <cell r="D2260">
-            <v>492.49561126113719</v>
+            <v>495.86956575069809</v>
           </cell>
           <cell r="E2260">
             <v>209.2328294040949</v>
+          </cell>
+        </row>
+        <row r="2261">
+          <cell r="A2261">
+            <v>44249</v>
+          </cell>
+          <cell r="D2261">
+            <v>490.92836344505719</v>
+          </cell>
+          <cell r="E2261">
+            <v>198.51992811079401</v>
           </cell>
         </row>
       </sheetData>
@@ -61175,7 +61198,7 @@
             <v>44197</v>
           </cell>
           <cell r="C110">
-            <v>494.03442088230048</v>
+            <v>490.2008555654474</v>
           </cell>
           <cell r="D110">
             <v>204.40321387038799</v>
@@ -61186,10 +61209,10 @@
             <v>44228</v>
           </cell>
           <cell r="C111">
-            <v>492.49561126113719</v>
+            <v>490.92836344505719</v>
           </cell>
           <cell r="D111">
-            <v>209.2328294040949</v>
+            <v>198.51992811079401</v>
           </cell>
         </row>
       </sheetData>
@@ -61208,7 +61231,7 @@
             <v>3714929530</v>
           </cell>
           <cell r="G2">
-            <v>0.44594160118704962</v>
+            <v>0.44157922994593263</v>
           </cell>
           <cell r="H2">
             <v>0.56032805836997823</v>
@@ -61228,7 +61251,7 @@
             <v>55737000</v>
           </cell>
           <cell r="G3">
-            <v>0.26563233582364709</v>
+            <v>0.27508010891412737</v>
           </cell>
           <cell r="H3">
             <v>2.965781714038454E-2</v>
@@ -61248,7 +61271,7 @@
             <v>339000000</v>
           </cell>
           <cell r="G4">
-            <v>6.3772928729853864E-2</v>
+            <v>6.2110276675833097E-2</v>
           </cell>
           <cell r="H4">
             <v>4.4674823921718211E-2</v>
@@ -61268,7 +61291,7 @@
             <v>902160000</v>
           </cell>
           <cell r="G5">
-            <v>5.1870521812547428E-2</v>
+            <v>5.0547434655360747E-2</v>
           </cell>
           <cell r="H5">
             <v>0.14416604095929181</v>
@@ -61288,7 +61311,7 @@
             <v>746598072</v>
           </cell>
           <cell r="G6">
-            <v>5.0121657557831122E-2</v>
+            <v>5.018229588233817E-2</v>
           </cell>
           <cell r="H6">
             <v>0.1058555437796873</v>
@@ -61308,7 +61331,7 @@
             <v>443781062</v>
           </cell>
           <cell r="G7">
-            <v>3.9800668158157901E-2</v>
+            <v>3.9129173899198538E-2</v>
           </cell>
           <cell r="H7">
             <v>8.5066596654456469E-2</v>
@@ -61328,7 +61351,7 @@
             <v>86371464</v>
           </cell>
           <cell r="G8">
-            <v>3.2746680769462758E-2</v>
+            <v>3.2161247099097387E-2</v>
           </cell>
           <cell r="H8">
             <v>9.9999999999999985E-3</v>
@@ -61348,7 +61371,7 @@
             <v>29787362</v>
           </cell>
           <cell r="G9">
-            <v>2.613960916092696E-2</v>
+            <v>2.5159701144226429E-2</v>
           </cell>
           <cell r="H9">
             <v>1.025111917448334E-2</v>
@@ -61368,7 +61391,7 @@
             <v>48067937</v>
           </cell>
           <cell r="G10">
-            <v>2.3973996800523319E-2</v>
+            <v>2.4050531783885581E-2</v>
           </cell>
           <cell r="H10">
             <v>9.9999999999999985E-3</v>
@@ -61386,7 +61409,7 @@
       <sheetData sheetId="11">
         <row r="2">
           <cell r="A2">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B2" t="str">
             <v>BNBR3.SA</v>
@@ -61400,7 +61423,7 @@
         </row>
         <row r="3">
           <cell r="A3">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B3" t="str">
             <v>COCE3.SA</v>
@@ -61414,7 +61437,7 @@
         </row>
         <row r="4">
           <cell r="A4">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B4" t="str">
             <v>COCE5.SA</v>
@@ -61428,7 +61451,7 @@
         </row>
         <row r="5">
           <cell r="A5">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B5" t="str">
             <v>GRND3.SA</v>
@@ -61442,7 +61465,7 @@
         </row>
         <row r="6">
           <cell r="A6">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B6" t="str">
             <v>MDIA3.SA</v>
@@ -61456,7 +61479,7 @@
         </row>
         <row r="7">
           <cell r="A7">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B7" t="str">
             <v>HAPV3.SA</v>
@@ -61470,7 +61493,7 @@
         </row>
         <row r="8">
           <cell r="A8">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B8" t="str">
             <v>ARCE</v>
@@ -61484,7 +61507,7 @@
         </row>
         <row r="9">
           <cell r="A9">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B9" t="str">
             <v>PGMN3.SA</v>
@@ -61498,7 +61521,7 @@
         </row>
         <row r="10">
           <cell r="A10">
-            <v>44246</v>
+            <v>44249</v>
           </cell>
           <cell r="B10" t="str">
             <v>AERI3.SA</v>
@@ -61817,7 +61840,7 @@
   <dimension ref="B2:P34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61892,19 +61915,19 @@
       </c>
       <c r="C4" s="5">
         <f>VLOOKUP($B4,[1]tab1_retorno_empresas!$B$1:$O$12,2,0)</f>
-        <v>2.3627884524209719E-2</v>
+        <v>-2.8782745868783929E-2</v>
       </c>
       <c r="D4" s="5">
         <f>VLOOKUP($B4,[1]tab1_retorno_empresas!$B$1:$O$12,3,0)</f>
-        <v>-4.6770489329955867E-3</v>
+        <v>-5.5638442324778208E-2</v>
       </c>
       <c r="E4" s="5">
         <f>VLOOKUP($B4,[1]tab1_retorno_empresas!$B$1:$O$12,4,0)</f>
-        <v>0.2423418145296283</v>
+        <v>0.17873284231670561</v>
       </c>
       <c r="F4" s="5">
         <f>VLOOKUP($B4,[1]tab1_retorno_empresas!$B$1:$O$12,5,0)</f>
-        <v>0.78134469412859087</v>
+        <v>0.69013830968167933</v>
       </c>
       <c r="G4" s="59">
         <v>0</v>
@@ -61952,19 +61975,19 @@
       </c>
       <c r="C5" s="8">
         <f>VLOOKUP($B5,[1]tab1_retorno_empresas!$B$1:$O$12,2,0)</f>
-        <v>-3.1147822016431852E-3</v>
+        <v>1.484101611309185E-3</v>
       </c>
       <c r="D5" s="8">
         <f>VLOOKUP($B5,[1]tab1_retorno_empresas!$B$1:$O$12,3,0)</f>
-        <v>3.2985275104042033E-2</v>
+        <v>2.969805004166215E-2</v>
       </c>
       <c r="E5" s="8">
         <f>VLOOKUP($B5,[1]tab1_retorno_empresas!$B$1:$O$12,4,0)</f>
-        <v>0.823260256374581</v>
+        <v>0.81745817288467659</v>
       </c>
       <c r="F5" s="8">
         <f>VLOOKUP($B5,[1]tab1_retorno_empresas!$B$1:$O$12,5,0)</f>
-        <v>1.1047236094480439</v>
+        <v>1.0980258371127469</v>
       </c>
       <c r="G5" s="60">
         <v>0</v>
@@ -62013,23 +62036,23 @@
       </c>
       <c r="C6" s="48">
         <f>[1]tab1_retorno_empresas!C4</f>
-        <v>-2.926491065922077E-2</v>
+        <v>-4.9653274608967291E-2</v>
       </c>
       <c r="D6" s="48">
         <f>[1]tab1_retorno_empresas!D4</f>
-        <v>-7.9078973684210574E-2</v>
+        <v>-9.8421092105263064E-2</v>
       </c>
       <c r="E6" s="48">
         <f>[1]tab1_retorno_empresas!E4</f>
-        <v>0.55533328888888867</v>
+        <v>0.52266659999999998</v>
       </c>
       <c r="F6" s="48">
         <f>[1]tab1_retorno_empresas!F4</f>
-        <v>1.473144893043989</v>
+        <v>1.421201392975314</v>
       </c>
       <c r="G6" s="48">
         <f>_xlfn.XLOOKUP($B6,tab4_contribuicao!$B$3:$B$11,tab4_contribuicao!$H$3:$H$11)</f>
-        <v>3.2746680769462758E-2</v>
+        <v>3.2161247099097387E-2</v>
       </c>
       <c r="H6" s="48">
         <f>[1]tab1_retorno_empresas!G4</f>
@@ -62091,7 +62114,7 @@
       </c>
       <c r="G7" s="48">
         <f>_xlfn.XLOOKUP($B7,tab4_contribuicao!$B$3:$B$11,tab4_contribuicao!$H$3:$H$11)</f>
-        <v>2.3973996800523319E-2</v>
+        <v>2.4050531783885581E-2</v>
       </c>
       <c r="H7" s="48">
         <f>[1]tab1_retorno_empresas!G5</f>
@@ -62137,23 +62160,23 @@
       </c>
       <c r="C8" s="48">
         <f>[1]tab1_retorno_empresas!C6</f>
-        <v>-2.5393384313068149E-2</v>
+        <v>-5.4259358758195757E-2</v>
       </c>
       <c r="D8" s="48">
         <f>[1]tab1_retorno_empresas!D6</f>
-        <v>-9.1666666666666674E-2</v>
+        <v>-0.1284999833333334</v>
       </c>
       <c r="E8" s="48">
         <f>[1]tab1_retorno_empresas!E6</f>
-        <v>-9.0909090909092605E-3</v>
+        <v>-4.9272709090909313E-2</v>
       </c>
       <c r="F8" s="48">
         <f>[1]tab1_retorno_empresas!F6</f>
-        <v>0.16577540106951871</v>
+        <v>0.1185026951871657</v>
       </c>
       <c r="G8" s="48">
         <f>_xlfn.XLOOKUP($B8,tab4_contribuicao!$B$3:$B$11,tab4_contribuicao!$H$3:$H$11)</f>
-        <v>2.613960916092696E-2</v>
+        <v>2.5159701144226429E-2</v>
       </c>
       <c r="H8" s="48">
         <f>[1]tab1_retorno_empresas!G6</f>
@@ -62199,23 +62222,23 @@
       </c>
       <c r="C9" s="48">
         <f>[1]tab1_retorno_empresas!C7</f>
-        <v>-1.156812339331614E-2</v>
+        <v>-3.1128404669260701E-2</v>
       </c>
       <c r="D9" s="48">
         <f>[1]tab1_retorno_empresas!D7</f>
-        <v>-8.2338902147971349E-2</v>
+        <v>-0.10859188544152749</v>
       </c>
       <c r="E9" s="48">
         <f>[1]tab1_retorno_empresas!E7</f>
-        <v>-0.11303344867358719</v>
+        <v>-0.1384083044982701</v>
       </c>
       <c r="F9" s="48">
         <f>[1]tab1_retorno_empresas!F7</f>
-        <v>0.15407709625198021</v>
+        <v>0.1210605863462018</v>
       </c>
       <c r="G9" s="48">
         <f>_xlfn.XLOOKUP($B9,tab4_contribuicao!$B$3:$B$11,tab4_contribuicao!$H$3:$H$11)</f>
-        <v>5.1870521812547428E-2</v>
+        <v>5.0547434655360747E-2</v>
       </c>
       <c r="H9" s="48">
         <f>[1]tab1_retorno_empresas!G7</f>
@@ -62261,23 +62284,23 @@
       </c>
       <c r="C10" s="48">
         <f>[1]tab1_retorno_empresas!C8</f>
-        <v>-2.2890778286460689E-3</v>
+        <v>-1.725275438794804E-2</v>
       </c>
       <c r="D10" s="48">
         <f>[1]tab1_retorno_empresas!D8</f>
-        <v>-0.1042278595352948</v>
+        <v>-0.13035818759958351</v>
       </c>
       <c r="E10" s="48">
         <f>[1]tab1_retorno_empresas!E8</f>
-        <v>-0.35057471264367812</v>
+        <v>-0.36951892294593452</v>
       </c>
       <c r="F10" s="48">
         <f>[1]tab1_retorno_empresas!F8</f>
-        <v>-0.3376989773907233</v>
+        <v>-0.35701878230128492</v>
       </c>
       <c r="G10" s="48">
         <f>_xlfn.XLOOKUP($B10,tab4_contribuicao!$B$3:$B$11,tab4_contribuicao!$H$3:$H$11)</f>
-        <v>6.3772928729853864E-2</v>
+        <v>6.2110276675833097E-2</v>
       </c>
       <c r="H10" s="48">
         <f>[1]tab1_retorno_empresas!G8</f>
@@ -62323,23 +62346,23 @@
       </c>
       <c r="C11" s="48">
         <f>[1]tab1_retorno_empresas!C9</f>
-        <v>-2.2413793103448151E-2</v>
+        <v>-2.213156668608041E-2</v>
       </c>
       <c r="D11" s="48">
         <f>[1]tab1_retorno_empresas!D9</f>
-        <v>0.1146788990825689</v>
+        <v>0.1002621887287025</v>
       </c>
       <c r="E11" s="48">
         <f>[1]tab1_retorno_empresas!E9</f>
-        <v>1.609696225836146</v>
+        <v>1.57594369438478</v>
       </c>
       <c r="F11" s="48">
         <f>[1]tab1_retorno_empresas!F9</f>
-        <v>2.081521739130435</v>
+        <v>2.0416668478260869</v>
       </c>
       <c r="G11" s="48">
         <f>_xlfn.XLOOKUP($B11,tab4_contribuicao!$B$3:$B$11,tab4_contribuicao!$H$3:$H$11)</f>
-        <v>0.44594160118704962</v>
+        <v>0.44157922994593263</v>
       </c>
       <c r="H11" s="6">
         <f>[1]tab1_retorno_empresas!G9</f>
@@ -62385,23 +62408,23 @@
       </c>
       <c r="C12" s="48">
         <f>[1]tab1_retorno_empresas!C10</f>
-        <v>0.1014074814136892</v>
+        <v>0.13695173309160041</v>
       </c>
       <c r="D12" s="48">
         <f>[1]tab1_retorno_empresas!D10</f>
-        <v>3.6490608118537222E-2</v>
+        <v>6.9939884302379518E-2</v>
       </c>
       <c r="E12" s="48">
         <f>[1]tab1_retorno_empresas!E10</f>
-        <v>1.122930353619811</v>
+        <v>1.1914408477440079</v>
       </c>
       <c r="F12" s="48">
         <f>[1]tab1_retorno_empresas!F10</f>
-        <v>1.3747996346313229</v>
+        <v>1.451438369452339</v>
       </c>
       <c r="G12" s="48">
         <f>_xlfn.XLOOKUP($B12,tab4_contribuicao!$B$3:$B$11,tab4_contribuicao!$H$3:$H$11)</f>
-        <v>0.26563233582364709</v>
+        <v>0.27508010891412737</v>
       </c>
       <c r="H12" s="6">
         <f>[1]tab1_retorno_empresas!G10</f>
@@ -62447,23 +62470,23 @@
       </c>
       <c r="C13" s="48">
         <f>[1]tab1_retorno_empresas!C11</f>
-        <v>-1.477832512315269E-2</v>
+        <v>-3.4482758620689613E-2</v>
       </c>
       <c r="D13" s="48">
         <f>[1]tab1_retorno_empresas!D11</f>
-        <v>0.1086474501108647</v>
+        <v>8.6474501108647628E-2</v>
       </c>
       <c r="E13" s="48">
         <f>[1]tab1_retorno_empresas!E11</f>
-        <v>6.6098081023453936E-2</v>
+        <v>4.4776119402985197E-2</v>
       </c>
       <c r="F13" s="48">
         <f>[1]tab1_retorno_empresas!F11</f>
-        <v>6.6098081023453936E-2</v>
+        <v>4.4776119402985197E-2</v>
       </c>
       <c r="G13" s="48">
         <f>_xlfn.XLOOKUP($B13,tab4_contribuicao!$B$3:$B$11,tab4_contribuicao!$H$3:$H$11)</f>
-        <v>3.9800668158157901E-2</v>
+        <v>3.9129173899198538E-2</v>
       </c>
       <c r="H13" s="6">
         <f>[1]tab1_retorno_empresas!G11</f>
@@ -62509,23 +62532,23 @@
       </c>
       <c r="C14" s="49">
         <f>[1]tab1_retorno_empresas!C12</f>
-        <v>-0.14527027027027031</v>
+        <v>-0.1469594594594594</v>
       </c>
       <c r="D14" s="49">
         <f>[1]tab1_retorno_empresas!D12</f>
-        <v>1.2000000000000011E-2</v>
+        <v>1.0000000000000011E-2</v>
       </c>
       <c r="E14" s="49">
         <f>[1]tab1_retorno_empresas!E12</f>
-        <v>0.51724137931034453</v>
+        <v>0.5142428785607196</v>
       </c>
       <c r="F14" s="49">
         <f>[1]tab1_retorno_empresas!F12</f>
-        <v>0.51724137931034453</v>
+        <v>0.5142428785607196</v>
       </c>
       <c r="G14" s="49">
         <f>_xlfn.XLOOKUP($B14,tab4_contribuicao!$B$3:$B$11,tab4_contribuicao!$H$3:$H$11)</f>
-        <v>5.0121657557831122E-2</v>
+        <v>5.018229588233817E-2</v>
       </c>
       <c r="H14" s="18">
         <f>[1]tab1_retorno_empresas!G12</f>
@@ -62739,19 +62762,19 @@
       </c>
       <c r="D5" s="12">
         <f>[1]tab2_risco_empresas!B$3</f>
-        <v>1.4800000000000001E-2</v>
+        <v>1.37E-2</v>
       </c>
       <c r="E5" s="12">
         <f>[1]tab2_risco_empresas!C$3</f>
-        <v>7.22E-2</v>
+        <v>7.2499999999999995E-2</v>
       </c>
       <c r="F5" s="6">
         <f>[1]tab2_risco_empresas!D$3</f>
-        <v>4.8783783783783781</v>
+        <v>5.2919708029197077</v>
       </c>
       <c r="G5" s="12">
         <f>[1]tab2_risco_empresas!E$3</f>
-        <v>5.1999999999999998E-3</v>
+        <v>5.3E-3</v>
       </c>
       <c r="H5" s="53">
         <f>[1]tab2_risco_empresas!F$3</f>
@@ -62805,16 +62828,16 @@
         <v>AERI3.SA</v>
       </c>
       <c r="D7" s="12">
-        <v>0.13469999999999999</v>
+        <v>0.13450000000000001</v>
       </c>
       <c r="E7" s="12">
-        <v>0.27989999999999998</v>
+        <v>0.28100000000000003</v>
       </c>
       <c r="F7" s="6">
-        <v>2.077951002227171</v>
+        <v>2.0892193308550189</v>
       </c>
       <c r="G7" s="13">
-        <v>7.8299999999999995E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="H7" s="20">
         <v>4</v>
@@ -62823,7 +62846,7 @@
         <v>0.50380000000000003</v>
       </c>
       <c r="J7" s="13">
-        <v>-0.14380000000000001</v>
+        <v>-0.14699999999999999</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
@@ -62831,16 +62854,16 @@
         <v>ARCE</v>
       </c>
       <c r="D8" s="12">
-        <v>3.9399999999999998E-2</v>
+        <v>4.0599999999999997E-2</v>
       </c>
       <c r="E8" s="12">
-        <v>0.14080000000000001</v>
+        <v>0.14149999999999999</v>
       </c>
       <c r="F8" s="6">
-        <v>3.5736040609137061</v>
+        <v>3.485221674876847</v>
       </c>
       <c r="G8" s="13">
-        <v>1.9800000000000002E-2</v>
+        <v>0.02</v>
       </c>
       <c r="H8" s="20">
         <v>29</v>
@@ -62857,16 +62880,16 @@
         <v>HAPV3.SA</v>
       </c>
       <c r="D9" s="12">
-        <v>3.85E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E9" s="12">
-        <v>0.10059999999999999</v>
+        <v>0.1002</v>
       </c>
       <c r="F9" s="6">
-        <v>2.6129870129870132</v>
+        <v>2.6368421052631579</v>
       </c>
       <c r="G9" s="13">
-        <v>1.01E-2</v>
+        <v>0.01</v>
       </c>
       <c r="H9" s="20">
         <v>34</v>
@@ -62883,16 +62906,16 @@
         <v>BNBR3.SA</v>
       </c>
       <c r="D10" s="12">
-        <v>2.69E-2</v>
+        <v>2.64E-2</v>
       </c>
       <c r="E10" s="12">
-        <v>0.13900000000000001</v>
+        <v>0.13919999999999999</v>
       </c>
       <c r="F10" s="6">
-        <v>5.1672862453531598</v>
+        <v>5.2727272727272734</v>
       </c>
       <c r="G10" s="13">
-        <v>1.9300000000000001E-2</v>
+        <v>1.9400000000000001E-2</v>
       </c>
       <c r="H10" s="20">
         <v>48</v>
@@ -62906,54 +62929,54 @@
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="str">
-        <v>PGMN3.SA</v>
+        <v>COCE3.SA</v>
       </c>
       <c r="D11" s="15">
-        <v>1.37E-2</v>
+        <v>1.17E-2</v>
       </c>
       <c r="E11" s="15">
-        <v>8.5000000000000006E-2</v>
+        <v>0.12909999999999999</v>
       </c>
       <c r="F11" s="16">
-        <v>6.2043795620437958</v>
+        <v>11.034188034188031</v>
       </c>
       <c r="G11" s="13">
-        <v>7.1999999999999998E-3</v>
+        <v>1.67E-2</v>
       </c>
       <c r="H11" s="20">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="I11" s="13">
-        <v>0.12970000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="J11" s="13">
-        <v>-0.1087</v>
+        <v>-0.28670000000000001</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="4" t="str">
-        <v>COCE3.SA</v>
+        <v>PGMN3.SA</v>
       </c>
       <c r="D12" s="15">
-        <v>1.17E-2</v>
+        <v>1.03E-2</v>
       </c>
       <c r="E12" s="15">
-        <v>0.12909999999999999</v>
+        <v>8.5199999999999998E-2</v>
       </c>
       <c r="F12" s="16">
-        <v>11.034188034188031</v>
+        <v>8.2718446601941746</v>
       </c>
       <c r="G12" s="13">
-        <v>1.67E-2</v>
+        <v>7.3000000000000001E-3</v>
       </c>
       <c r="H12" s="20">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I12" s="13">
-        <v>0.5</v>
+        <v>0.12529999999999999</v>
       </c>
       <c r="J12" s="13">
-        <v>-0.28670000000000001</v>
+        <v>-0.1087</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
@@ -62961,16 +62984,16 @@
         <v>GRND3.SA</v>
       </c>
       <c r="D13" s="15">
-        <v>6.3E-3</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="E13" s="15">
-        <v>7.9000000000000001E-2</v>
+        <v>7.9399999999999998E-2</v>
       </c>
       <c r="F13" s="16">
-        <v>12.53968253968254</v>
+        <v>13.92982456140351</v>
       </c>
       <c r="G13" s="13">
-        <v>6.1999999999999998E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="H13" s="20">
         <v>48</v>
@@ -62987,16 +63010,16 @@
         <v>COCE5.SA</v>
       </c>
       <c r="D14" s="15">
-        <v>5.5999999999999999E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="E14" s="15">
-        <v>6.7100000000000007E-2</v>
+        <v>6.7799999999999999E-2</v>
       </c>
       <c r="F14" s="16">
-        <v>11.982142857142859</v>
+        <v>14.125</v>
       </c>
       <c r="G14" s="13">
-        <v>4.4999999999999997E-3</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="H14" s="20">
         <v>48</v>
@@ -63013,16 +63036,16 @@
         <v>MDIA3.SA</v>
       </c>
       <c r="D15" s="17">
-        <v>-3.5000000000000001E-3</v>
+        <v>-4.1000000000000003E-3</v>
       </c>
       <c r="E15" s="17">
-        <v>9.2899999999999996E-2</v>
+        <v>9.3200000000000005E-2</v>
       </c>
       <c r="F15" s="18">
-        <v>-26.542857142857141</v>
+        <v>-22.73170731707317</v>
       </c>
       <c r="G15" s="19">
-        <v>8.6E-3</v>
+        <v>8.6999999999999994E-3</v>
       </c>
       <c r="H15" s="21">
         <v>48</v>
@@ -63054,7 +63077,7 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63102,19 +63125,19 @@
       </c>
       <c r="C4" s="23">
         <f>[1]tab3_risco_sistemico!B2</f>
-        <v>0.13070000000000001</v>
+        <v>0.13689999999999999</v>
       </c>
       <c r="D4" s="23">
         <f>[1]tab3_risco_sistemico!C2</f>
-        <v>1.03E-2</v>
+        <v>1.0699999999999999E-2</v>
       </c>
       <c r="E4" s="23">
         <f>[1]tab3_risco_sistemico!D2</f>
-        <v>0.505</v>
+        <v>0.50639999999999996</v>
       </c>
       <c r="F4" s="23">
         <f>[1]tab3_risco_sistemico!E2</f>
-        <v>0.55220000000000002</v>
+        <v>0.55630000000000002</v>
       </c>
       <c r="G4" s="23">
         <f>[1]tab3_risco_sistemico!F2</f>
@@ -63122,7 +63145,7 @@
       </c>
       <c r="H4" s="23">
         <f>[1]tab3_risco_sistemico!G2</f>
-        <v>0.30499999999999999</v>
+        <v>0.3095</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -63131,22 +63154,22 @@
         <v>ARCE_SP500</v>
       </c>
       <c r="C5" s="25">
-        <v>0.1348</v>
+        <v>0.1439</v>
       </c>
       <c r="D5" s="25">
-        <v>1.06E-2</v>
+        <v>1.1299999999999999E-2</v>
       </c>
       <c r="E5" s="25">
-        <v>1.0178</v>
+        <v>1.0202</v>
       </c>
       <c r="F5" s="26">
-        <v>0.43540000000000001</v>
+        <v>0.43409999999999999</v>
       </c>
       <c r="G5" s="25">
-        <v>1.6199999999999999E-2</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="H5" s="25">
-        <v>0.18959999999999999</v>
+        <v>0.18840000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -63154,22 +63177,22 @@
         <v>COCE3.SA</v>
       </c>
       <c r="C6" s="12">
-        <v>-1.0200000000000001E-2</v>
+        <v>-5.1999999999999998E-3</v>
       </c>
       <c r="D6" s="12">
-        <v>-8.9999999999999998E-4</v>
+        <v>-4.0000000000000002E-4</v>
       </c>
       <c r="E6" s="12">
-        <v>0.85019999999999996</v>
+        <v>0.88780000000000003</v>
       </c>
       <c r="F6" s="13">
-        <v>0.47570000000000001</v>
+        <v>0.4985</v>
       </c>
       <c r="G6" s="12">
-        <v>5.9999999999999995E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="H6" s="12">
-        <v>0.2263</v>
+        <v>0.2485</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -63177,22 +63200,22 @@
         <v>MDIA3.SA</v>
       </c>
       <c r="C7" s="12">
-        <v>-0.16209999999999999</v>
+        <v>-0.1595</v>
       </c>
       <c r="D7" s="12">
-        <v>-1.46E-2</v>
+        <v>-1.44E-2</v>
       </c>
       <c r="E7" s="12">
-        <v>0.75509999999999999</v>
+        <v>0.75419999999999998</v>
       </c>
       <c r="F7" s="13">
-        <v>0.58720000000000006</v>
+        <v>0.58650000000000002</v>
       </c>
       <c r="G7" s="12">
         <v>0</v>
       </c>
       <c r="H7" s="12">
-        <v>0.3448</v>
+        <v>0.34399999999999997</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -63200,22 +63223,22 @@
         <v>HAPV3.SA</v>
       </c>
       <c r="C8" s="12">
-        <v>0.42209999999999998</v>
+        <v>0.42970000000000003</v>
       </c>
       <c r="D8" s="12">
-        <v>2.98E-2</v>
+        <v>3.0200000000000001E-2</v>
       </c>
       <c r="E8" s="12">
-        <v>0.66790000000000005</v>
+        <v>0.68030000000000002</v>
       </c>
       <c r="F8" s="13">
-        <v>0.54139999999999999</v>
+        <v>0.55579999999999996</v>
       </c>
       <c r="G8" s="12">
-        <v>8.9999999999999998E-4</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="H8" s="12">
-        <v>0.29310000000000003</v>
+        <v>0.30890000000000001</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -63223,22 +63246,22 @@
         <v>GRND3.SA</v>
       </c>
       <c r="C9" s="15">
-        <v>-3.0700000000000002E-2</v>
+        <v>-3.0599999999999999E-2</v>
       </c>
       <c r="D9" s="15">
         <v>-2.5999999999999999E-3</v>
       </c>
       <c r="E9" s="15">
-        <v>0.6</v>
+        <v>0.60429999999999995</v>
       </c>
       <c r="F9" s="13">
-        <v>0.54820000000000002</v>
+        <v>0.55179999999999996</v>
       </c>
       <c r="G9" s="15">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="H9" s="15">
-        <v>0.30049999999999999</v>
+        <v>0.30449999999999999</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -63246,22 +63269,22 @@
         <v>COCE5.SA</v>
       </c>
       <c r="C10" s="12">
-        <v>-3.4599999999999999E-2</v>
+        <v>-3.8300000000000001E-2</v>
       </c>
       <c r="D10" s="12">
-        <v>-2.8999999999999998E-3</v>
+        <v>-3.2000000000000002E-3</v>
       </c>
       <c r="E10" s="12">
-        <v>0.57750000000000001</v>
+        <v>0.5867</v>
       </c>
       <c r="F10" s="13">
-        <v>0.62150000000000005</v>
+        <v>0.62739999999999996</v>
       </c>
       <c r="G10" s="12">
         <v>0</v>
       </c>
       <c r="H10" s="12">
-        <v>0.38629999999999998</v>
+        <v>0.39369999999999999</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -63269,22 +63292,22 @@
         <v>PGMN3.SA</v>
       </c>
       <c r="C11" s="12">
-        <v>-0.17519999999999999</v>
+        <v>-0.17430000000000001</v>
       </c>
       <c r="D11" s="12">
-        <v>-1.5900000000000001E-2</v>
+        <v>-1.5800000000000002E-2</v>
       </c>
       <c r="E11" s="12">
-        <v>0.41360000000000002</v>
+        <v>0.42349999999999999</v>
       </c>
       <c r="F11" s="13">
-        <v>0.33310000000000001</v>
+        <v>0.35520000000000002</v>
       </c>
       <c r="G11" s="12">
-        <v>0.51880000000000004</v>
+        <v>0.48970000000000002</v>
       </c>
       <c r="H11" s="12">
-        <v>0.1109</v>
+        <v>0.12609999999999999</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -63292,22 +63315,22 @@
         <v>BNBR3.SA</v>
       </c>
       <c r="C12" s="12">
-        <v>0.28439999999999999</v>
+        <v>0.28179999999999999</v>
       </c>
       <c r="D12" s="12">
-        <v>2.1100000000000001E-2</v>
+        <v>2.0899999999999998E-2</v>
       </c>
       <c r="E12" s="12">
-        <v>0.3921</v>
+        <v>0.4047</v>
       </c>
       <c r="F12" s="13">
-        <v>0.20369999999999999</v>
+        <v>0.21079999999999999</v>
       </c>
       <c r="G12" s="12">
-        <v>0.1648</v>
+        <v>0.15049999999999999</v>
       </c>
       <c r="H12" s="12">
-        <v>4.1500000000000002E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -63315,22 +63338,22 @@
         <v>ARCE_Ibovespa</v>
       </c>
       <c r="C13" s="17">
-        <v>0.54630000000000001</v>
+        <v>0.58040000000000003</v>
       </c>
       <c r="D13" s="17">
-        <v>3.6999999999999998E-2</v>
+        <v>3.8899999999999997E-2</v>
       </c>
       <c r="E13" s="17">
-        <v>0.13489999999999999</v>
+        <v>0.1085</v>
       </c>
       <c r="F13" s="19">
-        <v>7.9299999999999995E-2</v>
+        <v>6.3799999999999996E-2</v>
       </c>
       <c r="G13" s="17">
-        <v>0.68269999999999997</v>
+        <v>0.74239999999999995</v>
       </c>
       <c r="H13" s="17">
-        <v>6.3E-3</v>
+        <v>4.1000000000000003E-3</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -63439,7 +63462,7 @@
       </c>
       <c r="H3" s="31">
         <f>[1]contribuicao!G2</f>
-        <v>0.44594160118704962</v>
+        <v>0.44157922994593263</v>
       </c>
       <c r="I3" s="31">
         <f>[1]contribuicao!H2</f>
@@ -63472,7 +63495,7 @@
       </c>
       <c r="H4" s="31">
         <f>[1]contribuicao!G3</f>
-        <v>0.26563233582364709</v>
+        <v>0.27508010891412737</v>
       </c>
       <c r="I4" s="31">
         <f>[1]contribuicao!H3</f>
@@ -63505,7 +63528,7 @@
       </c>
       <c r="H5" s="31">
         <f>[1]contribuicao!G4</f>
-        <v>6.3772928729853864E-2</v>
+        <v>6.2110276675833097E-2</v>
       </c>
       <c r="I5" s="31">
         <f>[1]contribuicao!H4</f>
@@ -63538,7 +63561,7 @@
       </c>
       <c r="H6" s="31">
         <f>[1]contribuicao!G5</f>
-        <v>5.1870521812547428E-2</v>
+        <v>5.0547434655360747E-2</v>
       </c>
       <c r="I6" s="31">
         <f>[1]contribuicao!H5</f>
@@ -63571,7 +63594,7 @@
       </c>
       <c r="H7" s="31">
         <f>[1]contribuicao!G6</f>
-        <v>5.0121657557831122E-2</v>
+        <v>5.018229588233817E-2</v>
       </c>
       <c r="I7" s="31">
         <f>[1]contribuicao!H6</f>
@@ -63604,7 +63627,7 @@
       </c>
       <c r="H8" s="31">
         <f>[1]contribuicao!G7</f>
-        <v>3.9800668158157901E-2</v>
+        <v>3.9129173899198538E-2</v>
       </c>
       <c r="I8" s="31">
         <f>[1]contribuicao!H7</f>
@@ -63637,7 +63660,7 @@
       </c>
       <c r="H9" s="31">
         <f>[1]contribuicao!G8</f>
-        <v>3.2746680769462758E-2</v>
+        <v>3.2161247099097387E-2</v>
       </c>
       <c r="I9" s="31">
         <f>[1]contribuicao!H8</f>
@@ -63670,7 +63693,7 @@
       </c>
       <c r="H10" s="31">
         <f>[1]contribuicao!G9</f>
-        <v>2.613960916092696E-2</v>
+        <v>2.5159701144226429E-2</v>
       </c>
       <c r="I10" s="31">
         <f>[1]contribuicao!H9</f>
@@ -63703,7 +63726,7 @@
       </c>
       <c r="H11" s="31">
         <f>[1]contribuicao!G10</f>
-        <v>2.3973996800523319E-2</v>
+        <v>2.4050531783885581E-2</v>
       </c>
       <c r="I11" s="31">
         <f>[1]contribuicao!H10</f>
@@ -63730,7 +63753,7 @@
       </c>
       <c r="H12" s="34">
         <f>SUM(H3:H11)</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="I12" s="34">
         <f>SUM(I3:I11)</f>
@@ -63968,7 +63991,7 @@
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="43">
         <f>[1]data_inclusao!A2</f>
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="C4" t="str">
         <f>[1]data_inclusao!B2</f>
@@ -63986,7 +64009,7 @@
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="43">
         <f>[1]data_inclusao!A3</f>
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="C5" t="str">
         <f>[1]data_inclusao!B3</f>
@@ -64004,7 +64027,7 @@
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="43">
         <f>[1]data_inclusao!A4</f>
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="C6" t="str">
         <f>[1]data_inclusao!B4</f>
@@ -64022,7 +64045,7 @@
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="43">
         <f>[1]data_inclusao!A5</f>
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="C7" t="str">
         <f>[1]data_inclusao!B5</f>
@@ -64040,7 +64063,7 @@
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="43">
         <f>[1]data_inclusao!A6</f>
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="C8" t="str">
         <f>[1]data_inclusao!B6</f>
@@ -64058,7 +64081,7 @@
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="43">
         <f>[1]data_inclusao!A7</f>
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="C9" t="str">
         <f>[1]data_inclusao!B7</f>
@@ -64076,7 +64099,7 @@
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="43">
         <f>[1]data_inclusao!A8</f>
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="C10" t="str">
         <f>[1]data_inclusao!B8</f>
@@ -64094,7 +64117,7 @@
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="43">
         <f>[1]data_inclusao!A9</f>
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="C11" t="str">
         <f>[1]data_inclusao!B9</f>
@@ -64112,7 +64135,7 @@
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="44">
         <f>[1]data_inclusao!A10</f>
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="C12" s="40" t="str">
         <f>[1]data_inclusao!B10</f>

</xml_diff>